<commit_message>
- Replaced connector by the reference: C1509219 - Female header
- Modified boards to improve manufacturing and asembly: increased connector pad sizes
</commit_message>
<xml_diff>
--- a/Mitai - NearField_PCB_Probes/E-Field-Near-Filed Probe/Documents_Mi-tai/Assembly/BOM/Bill of Materials-NearField_E_Probe - JLCPCB.xlsx
+++ b/Mitai - NearField_PCB_Probes/E-Field-Near-Filed Probe/Documents_Mi-tai/Assembly/BOM/Bill of Materials-NearField_E_Probe - JLCPCB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\EE-PCB-Marketing\Mitai - NearField_PCB_Probes\E-Field-Near-Filed Probe\Documents\Assembly\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\EE-PCB-Marketing\Mitai - NearField_PCB_Probes\E-Field-Near-Filed Probe\Documents_Mi-tai\Assembly\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB4F928-738C-4EF4-8E5C-B07EEC8B1EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB17D2E-B3BA-4D60-8D8E-4D2A4DAD3A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Comment</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>RFSOLUTIONS_CON-SMA-EDGE-S</t>
+  </si>
+  <si>
+    <t>C1509219</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -555,7 +558,9 @@
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>